<commit_message>
updates to database code and API spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/APIs.xlsx
+++ b/documentation/APIs.xlsx
@@ -24,26 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
-  <si>
-    <t>Name:</t>
-  </si>
-  <si>
-    <t>Args:</t>
-  </si>
-  <si>
-    <t>Input format:</t>
-  </si>
-  <si>
-    <t>Returns:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Probable use level</t>
-  </si>
-  <si>
     <t>ACCESSION_SEARCH</t>
   </si>
   <si>
@@ -89,12 +74,6 @@
     <t>1 array of product names</t>
   </si>
   <si>
-    <t>SEARCH_RESULT</t>
-  </si>
-  <si>
-    <t>Accession number</t>
-  </si>
-  <si>
     <t>2 arrays, 1: list of accessions and 2: list of corresponding concatenated geneID, Product name and chromosome location</t>
   </si>
   <si>
@@ -168,6 +147,60 @@
   </si>
   <si>
     <t>Concatenates all of the protein sequences</t>
+  </si>
+  <si>
+    <t>top for middle</t>
+  </si>
+  <si>
+    <t>middle for top</t>
+  </si>
+  <si>
+    <t>middle for bottom</t>
+  </si>
+  <si>
+    <t>Uses DNA_sequence</t>
+  </si>
+  <si>
+    <t>Probable use levels</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Input format</t>
+  </si>
+  <si>
+    <t>Args</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SQL query on loci table, bridgeing chromosome locationto retreive location name</t>
+  </si>
+  <si>
+    <t>SQL query on loci table retreiving GeneID / GI numer</t>
+  </si>
+  <si>
+    <t>SQL query on loci table retreiving CDS_translated</t>
+  </si>
+  <si>
+    <t>SQL query on loci table retreiving DNA_sequence</t>
+  </si>
+  <si>
+    <t>INTRON-EXON-RESTRICTION_SITE_STRINGS</t>
+  </si>
+  <si>
+    <t>Uses CHROMOSOME_LOCATION,GENE_ID,PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>Accession numbers</t>
+  </si>
+  <si>
+    <t>1 array</t>
+  </si>
+  <si>
+    <t>SEARCH_RESULTS</t>
   </si>
 </sst>
 </file>
@@ -206,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -214,69 +247,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA3A3A3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA3A3A3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA3A3A3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA3A3A3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA3A3A3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA3A3A3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA3A3A3"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA3A3A3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA3A3A3"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA3A3A3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,285 +545,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="54.90625" customWidth="1"/>
+    <col min="5" max="6" width="61.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>